<commit_message>
Added excel plot and matlab file
</commit_message>
<xml_diff>
--- a/Lab 2 Clustering and PCA/KPlot.xlsx
+++ b/Lab 2 Clustering and PCA/KPlot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\lab2-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Year 4\lab2-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2F129A-C95D-4E70-B6C5-55D9D855CEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137491BA-6E1D-40E4-8C35-EA22A80B265D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="120" windowWidth="19200" windowHeight="12050" xr2:uid="{F3B1CDE3-B53D-478C-8DF8-8524211014F8}"/>
+    <workbookView xWindow="3270" yWindow="120" windowWidth="19200" windowHeight="12045" xr2:uid="{F3B1CDE3-B53D-478C-8DF8-8524211014F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,8 +145,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10787096255825165"/>
-          <c:y val="1.4725253847290537E-2"/>
+          <c:x val="0.10744271448401599"/>
+          <c:y val="1.4725328594626061E-2"/>
           <c:w val="0.8821038084525149"/>
           <c:h val="0.8469882417512824"/>
         </c:manualLayout>
@@ -1419,6 +1419,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Distortion[8]</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> vs K-Initial Centroids</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1573,6 +1603,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>K-Initial Centroids</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1638,6 +1723,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Distortion[8]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2871,15 +3011,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:colOff>281427</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>13447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>107016</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>116861</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3206,17 +3346,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F956B6-07B5-48C4-8055-E7F94B1E2D65}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -3248,7 +3388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3283,7 +3423,7 @@
         <v>5470.0698240000002</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3318,7 +3458,7 @@
         <v>3178.5273440000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3353,7 +3493,7 @@
         <v>3148.4338379999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3388,7 +3528,7 @@
         <v>3138.711914</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3423,7 +3563,7 @@
         <v>3132.9624020000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3458,7 +3598,7 @@
         <v>3119.7006839999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3493,7 +3633,7 @@
         <v>3107.3989259999998</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3528,7 +3668,7 @@
         <v>3105.0756839999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3563,7 +3703,7 @@
         <v>3104.7531739999999</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -3571,7 +3711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1</v>
       </c>
@@ -3579,7 +3719,7 @@
         <v>732439.625</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2</v>
       </c>
@@ -3587,7 +3727,7 @@
         <v>317257.1875</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>3</v>
       </c>
@@ -3595,7 +3735,7 @@
         <v>78126.726563000004</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>4</v>
       </c>
@@ -3603,7 +3743,7 @@
         <v>32335.771484000001</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>5</v>
       </c>
@@ -3611,7 +3751,7 @@
         <v>13455.113281</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>6</v>
       </c>
@@ -3619,7 +3759,7 @@
         <v>5021.8203130000002</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>7</v>
       </c>
@@ -3627,7 +3767,7 @@
         <v>4581.7456050000001</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>8</v>
       </c>
@@ -3635,7 +3775,7 @@
         <v>3987.8354490000002</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>9</v>
       </c>
@@ -3643,7 +3783,7 @@
         <v>3529.085693</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>10</v>
       </c>

</xml_diff>